<commit_message>
project-guide lines and test case template added
</commit_message>
<xml_diff>
--- a/Teams.xlsx
+++ b/Teams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIHT\cg\02batch05042021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD648D8-E13F-477F-87B2-E6D420B2D1F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A986417-BA85-49F2-A2B1-A38AB7F83E11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6D5692CA-8987-4F28-9638-79F47074A2C5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="77">
   <si>
     <t>Arpit Jain</t>
   </si>
@@ -260,13 +260,19 @@
   </si>
   <si>
     <t>Shfted from Team-2</t>
+  </si>
+  <si>
+    <t>Applied Sick Leave</t>
+  </si>
+  <si>
+    <t>Batch disolved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +306,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -343,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -353,6 +366,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1988,10 +2002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F93B5B-B787-4B95-A518-6BED4AA4DACF}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2011,7 +2025,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2055,6 +2069,9 @@
       <c r="C7" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="F7" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="6"/>
@@ -2071,7 +2088,7 @@
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2107,7 +2124,7 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2123,7 +2140,7 @@
       <c r="A18">
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
@@ -2153,10 +2170,10 @@
       <c r="A21">
         <v>12</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2172,7 +2189,7 @@
       <c r="A25">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -2221,7 +2238,7 @@
       <c r="A32">
         <v>17</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -2234,39 +2251,49 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>18</v>
-      </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>19</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>20</v>
-      </c>
-      <c r="C35" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C35" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>45</v>
       </c>
@@ -2274,11 +2301,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>22</v>
-      </c>
-      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -2291,23 +2318,23 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
         <v>46</v>
       </c>
@@ -2315,8 +2342,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -2329,17 +2359,24 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>24</v>
+      </c>
       <c r="C48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>25</v>
+      </c>
       <c r="C49" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>